<commit_message>
Heat-Abatement Excell is done but not migrating in the evaluations yet
</commit_message>
<xml_diff>
--- a/Excell_files/Locators.xlsx
+++ b/Excell_files/Locators.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammad Abbas Khan\source\repos\Automation-Zinpro\Excell_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB07420-7402-4969-B6A7-79E22F6396F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE45A7B-2DFA-4A4A-8390-EDA0B26D0D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Locomotion" sheetId="1" r:id="rId1"/>
+    <sheet name="HeatAbatement" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">HeatAbatement!$A$8:$N$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Locomotion!$F$7:$G$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>Closed</t>
   </si>
@@ -124,12 +126,82 @@
   <si>
     <t>L O C O M O T I O N    (Assesor Details)</t>
   </si>
+  <si>
+    <t>H E A T  --- A B A T E M E N T</t>
+  </si>
+  <si>
+    <t>Is drinking water readily available to cows exiting the milking parlor?</t>
+  </si>
+  <si>
+    <t>Is the area around the water trough free of mud, stones, etc?</t>
+  </si>
+  <si>
+    <t>Are fans located in the Feed Bunk Area?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Lactating</t>
+  </si>
+  <si>
+    <t>Accessible Water Trough Perimeter in Pen (cm)</t>
+  </si>
+  <si>
+    <t>Are HVLS Fans used (high volume, low speed)?</t>
+  </si>
+  <si>
+    <t>Temperature Fans Activate (°C)</t>
+  </si>
+  <si>
+    <t>Spacing (m)</t>
+  </si>
+  <si>
+    <t>Are fans located in the resting area/paddock?</t>
+  </si>
+  <si>
+    <t>Fans
+Feed Bunk Area</t>
+  </si>
+  <si>
+    <t>Resting Area/Padd-Lock</t>
+  </si>
+  <si>
+    <t>Soakers/Misters</t>
+  </si>
+  <si>
+    <t>Are soakers/misters located in the Feed Bunk Area?</t>
+  </si>
+  <si>
+    <t>Are there soakers/misters located in the Resting Area/Paddock?</t>
+  </si>
+  <si>
+    <t>Does water droplet effectively soak cows?</t>
+  </si>
+  <si>
+    <t>Does the frequency of soaking vary depending upon temperature?</t>
+  </si>
+  <si>
+    <t>Shade</t>
+  </si>
+  <si>
+    <t>Is there shade over the Feed Bunk Area?</t>
+  </si>
+  <si>
+    <t>Is there shade over the Resting Area/Paddock?</t>
+  </si>
+  <si>
+    <t>Are air cooling units such as Shade-Tracker or Koral-Kool used below shade?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +247,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +278,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -353,53 +447,425 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,209 +1154,209 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="K7" s="14"/>
+      <c r="L7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10">
         <v>9</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="12">
+      <c r="G8" s="11"/>
+      <c r="H8" s="10">
         <v>22</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="12">
+      <c r="I8" s="12"/>
+      <c r="J8" s="10">
         <v>1</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="1">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="7">
         <v>8</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="1">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="12">
+      <c r="G9" s="9"/>
+      <c r="H9" s="7">
+        <v>15</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="7">
         <v>2</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="1">
+      <c r="K9" s="9"/>
+      <c r="L9" s="8">
         <v>1</v>
       </c>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="1">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7">
         <v>7</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="1">
+      <c r="G10" s="9"/>
+      <c r="H10" s="7">
         <v>2</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="12">
+      <c r="I10" s="8"/>
+      <c r="J10" s="7">
         <v>3</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="1">
+      <c r="K10" s="9"/>
+      <c r="L10" s="8">
         <v>5</v>
       </c>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="1">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7">
         <v>6</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1">
+      <c r="G11" s="9"/>
+      <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="12">
+      <c r="I11" s="8"/>
+      <c r="J11" s="7">
         <v>4</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="1">
+      <c r="K11" s="9"/>
+      <c r="L11" s="8">
         <v>8</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="15">
         <v>5</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3">
+      <c r="G12" s="16"/>
+      <c r="H12" s="15">
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="12">
+      <c r="I12" s="17"/>
+      <c r="J12" s="15">
         <v>5</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="3">
+      <c r="K12" s="16"/>
+      <c r="L12" s="17">
         <v>9</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -900,14 +1366,15 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="H9:I9"/>
@@ -924,9 +1391,866 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B3B943-692A-477B-A890-606E2E65BCE5}">
+  <dimension ref="A5:O44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="60"/>
+      <c r="I8" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="60"/>
+      <c r="K8" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="57"/>
+      <c r="M8" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="57"/>
+    </row>
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="43"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="48"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="50"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="52"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="24"/>
+      <c r="M15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="43"/>
+    </row>
+    <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="43"/>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="24"/>
+      <c r="M23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
+    </row>
+    <row r="25" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="24"/>
+      <c r="I29" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="25"/>
+      <c r="M29" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29" s="41"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="24"/>
+      <c r="I30" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="24"/>
+      <c r="K30" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="25"/>
+      <c r="M30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="27"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="24"/>
+      <c r="I31" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="27"/>
+    </row>
+    <row r="32" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="46"/>
+    </row>
+    <row r="33" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="46"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="24"/>
+      <c r="I34" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="24"/>
+      <c r="K34" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="25"/>
+      <c r="M34" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="27"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="24"/>
+      <c r="K38" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="25"/>
+      <c r="M38" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="41"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="24"/>
+      <c r="I39" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="24"/>
+      <c r="K39" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" s="25"/>
+      <c r="M39" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" s="27"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="32"/>
+      <c r="I40" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="32"/>
+      <c r="K40" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" s="33"/>
+      <c r="M40" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40" s="35"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="110">
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A12:N14"/>
+    <mergeCell ref="A19:N21"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="A26:N28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="A5:N6"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="A35:N37"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="G34:H34"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:N11 G38:N40 G22:N23 G29:N31 G34:N34 G15:N16" xr:uid="{DF223E89-D9BA-46EC-A28F-99B537403C79}">
+      <formula1>$A$43:$A$44</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>